<commit_message>
Fixes a test case
</commit_message>
<xml_diff>
--- a/Docs/Lab04_WBT_TCs_Form.xlsx
+++ b/Docs/Lab04_WBT_TCs_Form.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="130">
   <si>
     <t xml:space="preserve">VVTA, PPFDP Informatica, 2021-2022</t>
   </si>
@@ -148,6 +148,7 @@
         <color rgb="FF0033B3"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">public void </t>
     </r>
@@ -157,6 +158,7 @@
         <color rgb="FF00627A"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">modifyEmployeeFunction</t>
     </r>
@@ -166,6 +168,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -175,6 +178,7 @@
         <color rgb="FF000000"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Employee </t>
     </r>
@@ -184,6 +188,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">employee, </t>
     </r>
@@ -193,6 +198,7 @@
         <color rgb="FF000000"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DidacticFunction </t>
     </r>
@@ -202,6 +208,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">newFunction) {</t>
     </r>
@@ -240,6 +247,7 @@
         <color rgb="FF0033B3"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">           if </t>
     </r>
@@ -249,6 +257,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(employee!=</t>
     </r>
@@ -258,6 +267,7 @@
         <color rgb="FF0033B3"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">null</t>
     </r>
@@ -267,6 +277,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">) {</t>
     </r>
@@ -305,6 +316,7 @@
         <color rgb="FF0033B3"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">               int </t>
     </r>
@@ -314,6 +326,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">i = </t>
     </r>
@@ -323,6 +336,7 @@
         <color rgb="FF1750EB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0</t>
     </r>
@@ -332,6 +346,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">;</t>
     </r>
@@ -343,6 +358,7 @@
         <color rgb="FF0033B3"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">               while </t>
     </r>
@@ -352,6 +368,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(i &lt; </t>
     </r>
@@ -361,6 +378,7 @@
         <color rgb="FF871094"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">employeeList</t>
     </r>
@@ -370,6 +388,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.size()) {</t>
     </r>
@@ -381,6 +400,7 @@
         <color rgb="FF0033B3"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">                      if </t>
     </r>
@@ -390,6 +410,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -399,6 +420,7 @@
         <color rgb="FF871094"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">employeeList</t>
     </r>
@@ -408,6 +430,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.get(i).getEmployeeId() == employee.getEmployeeId())</t>
     </r>
@@ -422,6 +445,7 @@
         <color rgb="FF871094"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">                            employeeList</t>
     </r>
@@ -431,6 +455,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.get(i).setFunction(newFunction);</t>
     </r>
@@ -529,6 +554,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">employee!=</t>
     </r>
@@ -538,6 +564,7 @@
         <color rgb="FF0033B3"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">null </t>
     </r>
@@ -561,6 +588,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">i &lt; </t>
     </r>
@@ -570,6 +598,7 @@
         <color rgb="FF871094"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">employeeList</t>
     </r>
@@ -579,6 +608,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.size()</t>
     </r>
@@ -602,6 +632,7 @@
         <color rgb="FF871094"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">employeeList</t>
     </r>
@@ -611,6 +642,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.get(i).getEmployeeId() == employee.getEmployeeId()</t>
     </r>
@@ -719,6 +751,9 @@
   </si>
   <si>
     <t xml:space="preserve">actual result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">Mariana, Hutanu, 1234567890876, Lecturer, 2500, 10</t>
@@ -1032,13 +1067,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
+    <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1113,47 +1149,47 @@
       <color rgb="FF0033B3"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF00627A"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF080808"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF1750EB"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF871094"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="28"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -1173,13 +1209,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <i val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1193,12 +1222,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1230,6 +1253,7 @@
       <charset val="238"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Candara"/>
@@ -1243,13 +1267,6 @@
       <name val="Candara"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1554,7 +1571,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="98">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1655,14 +1672,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1671,7 +1680,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1687,91 +1696,79 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="20" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1779,11 +1776,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1791,16 +1788,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1831,7 +1824,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1839,23 +1832,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1867,7 +1860,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1935,7 +1928,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1943,11 +1936,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="12" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="12" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="12" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="12" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1959,15 +1952,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="12" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="12" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="12" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2054,9 +2047,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>768600</xdr:colOff>
+      <xdr:colOff>768240</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:rowOff>5040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2069,8 +2062,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7811640" y="1466280"/>
-          <a:ext cx="5513400" cy="5987520"/>
+          <a:off x="7813440" y="1466280"/>
+          <a:ext cx="5513040" cy="5987160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2091,19 +2084,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>660960</xdr:colOff>
+      <xdr:colOff>660600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="1" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9717120" y="5564520"/>
-          <a:ext cx="335160" cy="420840"/>
+          <a:off x="9719280" y="5564520"/>
+          <a:ext cx="334800" cy="394200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2113,11 +2106,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2800" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
@@ -2141,19 +2145,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>542160</xdr:colOff>
+      <xdr:colOff>541800</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>110880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8807400" y="4536360"/>
-          <a:ext cx="335160" cy="394200"/>
+          <a:off x="8809200" y="4536360"/>
+          <a:ext cx="334800" cy="393840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2163,11 +2167,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2800" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
@@ -2191,19 +2206,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>113040</xdr:colOff>
+      <xdr:colOff>112680</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>26280</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11594880" y="3399840"/>
-          <a:ext cx="283320" cy="394200"/>
+          <a:off x="11596680" y="3399840"/>
+          <a:ext cx="282960" cy="393840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2213,11 +2228,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2800" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
@@ -2241,19 +2267,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>749160</xdr:colOff>
+      <xdr:colOff>748800</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11348640" y="5664240"/>
-          <a:ext cx="374400" cy="394200"/>
+          <a:off x="11350440" y="5664240"/>
+          <a:ext cx="374040" cy="393840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2263,11 +2289,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2800" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
@@ -2293,11 +2330,11 @@
   </sheetPr>
   <dimension ref="B1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
@@ -2508,7 +2545,7 @@
   </sheetPr>
   <dimension ref="B1:R38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E13" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2798,11 +2835,11 @@
       <c r="O17" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="P17" s="25" t="s">
+      <c r="P17" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="16" t="n">
@@ -2818,14 +2855,14 @@
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
-      <c r="O18" s="26" t="s">
+      <c r="O18" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="P18" s="25" t="s">
+      <c r="P18" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="16" t="n">
@@ -3018,35 +3055,35 @@
   </sheetPr>
   <dimension ref="B1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="9.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="18.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="18.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="27" width="46.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="27" width="22.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="27" width="8.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="27" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="27" width="11.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="27" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="27" width="25.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="27" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="27" width="7.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="27" width="8.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="15" style="27" width="9.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="27" width="4.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="27" width="4.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="27" width="5.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="27" width="4.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="27" width="4.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="27" width="5.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="27" width="5.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="24" style="27" width="9.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="9.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="18.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="18.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="46.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="25" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="25" width="8.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="25" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="11.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="25" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="25" width="25.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="25" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="25" width="7.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="25" width="8.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="15" style="25" width="9.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="25" width="4.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="25" width="4.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="25" width="5.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="25" width="4.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="25" width="4.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="25" width="5.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="25" width="5.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="24" style="25" width="9.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3059,411 +3096,411 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="27" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-      <c r="J3" s="31"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="27"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34" t="s">
+      <c r="D6" s="32"/>
+      <c r="E6" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34"/>
-      <c r="W6" s="34"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="32"/>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="33" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="36" t="s">
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="37" t="s">
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="33"/>
-      <c r="C8" s="38" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="40" t="s">
+      <c r="F8" s="31"/>
+      <c r="G8" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40" t="s">
+      <c r="H8" s="37"/>
+      <c r="I8" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="40"/>
-      <c r="K8" s="41" t="s">
+      <c r="J8" s="37"/>
+      <c r="K8" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="L8" s="41"/>
-      <c r="M8" s="36" t="s">
+      <c r="L8" s="38"/>
+      <c r="M8" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="N8" s="36" t="s">
+      <c r="N8" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="36" t="s">
+      <c r="O8" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="36" t="s">
+      <c r="P8" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="Q8" s="37" t="n">
+      <c r="Q8" s="35" t="n">
         <v>0</v>
       </c>
-      <c r="R8" s="37" t="n">
+      <c r="R8" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="S8" s="37" t="n">
+      <c r="S8" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="T8" s="37" t="s">
+      <c r="T8" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="U8" s="37" t="s">
+      <c r="U8" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="V8" s="37" t="s">
+      <c r="V8" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="W8" s="37" t="s">
+      <c r="W8" s="35" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="33"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="35" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="35" t="s">
+      <c r="K9" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="L9" s="35" t="s">
+      <c r="L9" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="46" t="s">
+      <c r="J10" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="K10" s="46" t="s">
+      <c r="K10" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="L10" s="46" t="s">
+      <c r="L10" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="M10" s="47" t="s">
+      <c r="M10" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="N10" s="47" t="s">
+      <c r="N10" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="O10" s="47" t="s">
+      <c r="O10" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="P10" s="47" t="s">
+      <c r="P10" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="Q10" s="48" t="s">
+      <c r="Q10" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="R10" s="49"/>
-      <c r="S10" s="49"/>
-      <c r="T10" s="49"/>
-      <c r="U10" s="49"/>
-      <c r="V10" s="49"/>
-      <c r="W10" s="49"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="45"/>
+      <c r="U10" s="45"/>
+      <c r="V10" s="45"/>
+      <c r="W10" s="45"/>
     </row>
     <row r="11" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="46" t="s">
+      <c r="G11" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="46" t="s">
+      <c r="I11" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="46" t="s">
+      <c r="J11" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="46" t="s">
+      <c r="K11" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="L11" s="46" t="s">
+      <c r="L11" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="M11" s="47" t="s">
+      <c r="M11" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="N11" s="47" t="s">
+      <c r="N11" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="O11" s="47" t="s">
+      <c r="O11" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="P11" s="47" t="s">
+      <c r="P11" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="49"/>
-      <c r="U11" s="48" t="s">
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="V11" s="49"/>
-      <c r="W11" s="49"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="45"/>
     </row>
     <row r="12" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="53" t="s">
+      <c r="E12" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="51" t="s">
+      <c r="F12" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="46" t="s">
+      <c r="H12" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="I12" s="46" t="s">
+      <c r="I12" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="46" t="s">
+      <c r="J12" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="K12" s="46" t="s">
+      <c r="K12" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="L12" s="46" t="s">
+      <c r="L12" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="M12" s="47" t="s">
+      <c r="M12" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="N12" s="47" t="s">
+      <c r="N12" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="O12" s="47" t="s">
+      <c r="O12" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="P12" s="47" t="s">
+      <c r="P12" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="49"/>
-      <c r="S12" s="49"/>
-      <c r="T12" s="49"/>
-      <c r="U12" s="48" t="s">
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="V12" s="49"/>
-      <c r="W12" s="49"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="45"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="27"/>
+      <c r="D13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="55"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="50"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="57" t="s">
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59" t="s">
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="60" t="s">
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="55"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="26" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="9" t="s">
@@ -3471,42 +3508,32 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="61" t="s">
+      <c r="E22" s="25" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E23" s="61" t="s">
+      <c r="E23" s="25" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E24" s="61" t="s">
+      <c r="E24" s="25" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E25" s="61" t="s">
+      <c r="E25" s="25" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="61" t="s">
+      <c r="E26" s="25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="61"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="61"/>
-    </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="61"/>
       <c r="F29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="61"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3562,27 +3589,27 @@
   </sheetPr>
   <dimension ref="B1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="24.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1"/>
-      <c r="C1" s="62"/>
+      <c r="C1" s="56"/>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3592,115 +3619,119 @@
       <c r="H1" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="66"/>
-      <c r="F4" s="67" t="s">
+      <c r="E4" s="60"/>
+      <c r="F4" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="67"/>
+      <c r="G4" s="61"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="68" t="s">
+      <c r="B5" s="58"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="62" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="69" t="n">
+      <c r="B6" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="70" t="n">
+      <c r="C6" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="71"/>
-      <c r="G6" s="69"/>
+      <c r="F6" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="66" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="69" t="n">
+      <c r="B7" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="70" t="n">
+      <c r="C7" s="64" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="50" t="s">
+      <c r="D7" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="72" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="69" t="s">
+      <c r="F7" s="67" t="s">
         <v>108</v>
       </c>
+      <c r="G7" s="63" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="69" t="n">
+      <c r="B8" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="70" t="n">
+      <c r="C8" s="64" t="n">
         <v>3</v>
       </c>
-      <c r="D8" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="50" t="s">
+      <c r="D8" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="73" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" s="69" t="s">
+      <c r="F8" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="63" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="74"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="76" t="s">
-        <v>111</v>
+      <c r="B11" s="70" t="s">
+        <v>112</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -3710,141 +3741,141 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="78"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="72"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="79" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="79"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="80" t="s">
+      <c r="B12" s="73" t="s">
         <v>113</v>
       </c>
-      <c r="H12" s="80"/>
-      <c r="I12" s="81" t="s">
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="82" t="s">
+      <c r="H12" s="74"/>
+      <c r="I12" s="75" t="s">
         <v>115</v>
       </c>
-      <c r="O12" s="82"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="O12" s="76"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="83" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" s="84" t="s">
+      <c r="B13" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="C13" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="84"/>
-      <c r="F13" s="85" t="s">
+      <c r="D13" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="86" t="s">
+      <c r="E13" s="78"/>
+      <c r="F13" s="79" t="s">
         <v>120</v>
       </c>
-      <c r="H13" s="87" t="s">
+      <c r="G13" s="80" t="s">
         <v>121</v>
       </c>
-      <c r="I13" s="83" t="s">
+      <c r="H13" s="81" t="s">
         <v>122</v>
       </c>
-      <c r="J13" s="84" t="s">
-        <v>116</v>
-      </c>
-      <c r="K13" s="84" t="s">
+      <c r="I13" s="77" t="s">
+        <v>123</v>
+      </c>
+      <c r="J13" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="L13" s="88" t="s">
-        <v>123</v>
-      </c>
-      <c r="M13" s="89" t="s">
+      <c r="K13" s="78" t="s">
+        <v>118</v>
+      </c>
+      <c r="L13" s="82" t="s">
         <v>124</v>
       </c>
-      <c r="N13" s="90" t="s">
+      <c r="M13" s="83" t="s">
         <v>125</v>
       </c>
-      <c r="O13" s="91" t="s">
+      <c r="N13" s="84" t="s">
         <v>126</v>
       </c>
+      <c r="O13" s="85" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="83"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="88"/>
-      <c r="M14" s="89"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="91"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="83"/>
+      <c r="N14" s="84"/>
+      <c r="O14" s="85"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="93" t="n">
+      <c r="B15" s="87" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="88" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="88" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="94" t="n">
+      <c r="E15" s="88"/>
+      <c r="F15" s="89" t="n">
+        <f aca="false">(9*100)/11</f>
+        <v>81.8181818181818</v>
+      </c>
+      <c r="G15" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="91" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" s="92" t="s">
+        <v>128</v>
+      </c>
+      <c r="J15" s="87" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" s="88" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" s="93" t="n">
         <v>0</v>
       </c>
-      <c r="D15" s="94" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95" t="n">
-        <f aca="false"> (9*100)/11</f>
-        <v>81.8181818181818</v>
-      </c>
-      <c r="G15" s="96" t="n">
-        <v>2</v>
-      </c>
-      <c r="H15" s="97" t="n">
-        <v>2</v>
-      </c>
-      <c r="I15" s="98" t="s">
-        <v>127</v>
-      </c>
-      <c r="J15" s="93" t="n">
-        <v>2</v>
-      </c>
-      <c r="K15" s="94" t="n">
-        <v>2</v>
-      </c>
-      <c r="L15" s="99" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="100" t="n">
+      <c r="M15" s="94" t="n">
         <v>100</v>
       </c>
-      <c r="N15" s="101" t="s">
-        <v>128</v>
-      </c>
-      <c r="O15" s="102" t="n">
+      <c r="N15" s="95" t="s">
+        <v>129</v>
+      </c>
+      <c r="O15" s="96" t="n">
         <f aca="false">C15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="103"/>
+      <c r="F16" s="97"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Move all files in repo
</commit_message>
<xml_diff>
--- a/Docs/Lab04_WBT_TCs_Form.xlsx
+++ b/Docs/Lab04_WBT_TCs_Form.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
   <si>
     <t xml:space="preserve">VVTA, PPFDP Informatica, 2021-2022</t>
   </si>
@@ -678,6 +678,9 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
+    <t xml:space="preserve">1-2-10</t>
+  </si>
+  <si>
     <t xml:space="preserve">*</t>
   </si>
   <si>
@@ -687,6 +690,9 @@
     <t xml:space="preserve">Mariana, Hutanu, 1234567890876, Lecturer, 2500, 6</t>
   </si>
   <si>
+    <t xml:space="preserve">1-2-3-4-5-7-8-4-9-10</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC03</t>
   </si>
   <si>
@@ -696,6 +702,9 @@
     <t xml:space="preserve">Mihaela;Pacuraru;1234567890876;Conferentiar;2600;3 </t>
   </si>
   <si>
+    <t xml:space="preserve">1-2-3-4-5-6-7-8-4-9-10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Remarks</t>
   </si>
   <si>
@@ -753,7 +762,7 @@
     <t xml:space="preserve">actual result</t>
   </si>
   <si>
-    <t xml:space="preserve">False</t>
+    <t xml:space="preserve">niciun employee nu are functia Conferentiar</t>
   </si>
   <si>
     <t xml:space="preserve">Mariana, Hutanu, 1234567890876, Lecturer, 2500, 10</t>
@@ -1074,7 +1083,7 @@
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1259,6 +1268,13 @@
       <name val="Candara"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Candara"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1836,11 +1852,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1936,11 +1952,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="12" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="12" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="12" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="12" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1952,7 +1968,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="12" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="12" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1960,7 +1976,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2047,9 +2063,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>768240</xdr:colOff>
+      <xdr:colOff>767880</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2063,7 +2079,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7813440" y="1466280"/>
-          <a:ext cx="5513040" cy="5987160"/>
+          <a:ext cx="5512680" cy="5986800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2084,9 +2100,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>660600</xdr:colOff>
+      <xdr:colOff>660240</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2096,7 +2112,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9719280" y="5564520"/>
-          <a:ext cx="334800" cy="394200"/>
+          <a:ext cx="334440" cy="393840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2145,9 +2161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541440</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2157,7 +2173,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8809200" y="4536360"/>
-          <a:ext cx="334800" cy="393840"/>
+          <a:ext cx="334440" cy="393480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2206,9 +2222,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>112680</xdr:colOff>
+      <xdr:colOff>112320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2218,7 +2234,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11596680" y="3399840"/>
-          <a:ext cx="282960" cy="393840"/>
+          <a:ext cx="282600" cy="393480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2267,9 +2283,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>748800</xdr:colOff>
+      <xdr:colOff>748440</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2279,7 +2295,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11350440" y="5664240"/>
-          <a:ext cx="374040" cy="393840"/>
+          <a:ext cx="373680" cy="393480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2545,7 +2561,7 @@
   </sheetPr>
   <dimension ref="B1:R38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3055,8 +3071,8 @@
   </sheetPr>
   <dimension ref="B1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3289,13 +3305,13 @@
         <v>80</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="G10" s="42" t="s">
         <v>80</v>
       </c>
       <c r="H10" s="42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I10" s="42" t="s">
         <v>80</v>
@@ -3310,7 +3326,7 @@
         <v>80</v>
       </c>
       <c r="M10" s="43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N10" s="43" t="s">
         <v>80</v>
@@ -3322,7 +3338,7 @@
         <v>80</v>
       </c>
       <c r="Q10" s="44" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="R10" s="45"/>
       <c r="S10" s="45"/>
@@ -3333,10 +3349,10 @@
     </row>
     <row r="11" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="39" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>79</v>
@@ -3345,34 +3361,34 @@
         <v>80</v>
       </c>
       <c r="F11" s="46" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H11" s="42" t="s">
         <v>80</v>
       </c>
       <c r="I11" s="42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J11" s="42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K11" s="42" t="s">
         <v>80</v>
       </c>
       <c r="L11" s="42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M11" s="43" t="s">
         <v>80</v>
       </c>
       <c r="N11" s="43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O11" s="43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P11" s="43" t="s">
         <v>80</v>
@@ -3382,63 +3398,63 @@
       <c r="S11" s="45"/>
       <c r="T11" s="45"/>
       <c r="U11" s="44" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="V11" s="45"/>
       <c r="W11" s="45"/>
     </row>
     <row r="12" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="39" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>79</v>
       </c>
       <c r="E12" s="48" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H12" s="42" t="s">
         <v>80</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J12" s="42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K12" s="42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L12" s="42" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M12" s="43" t="s">
         <v>80</v>
       </c>
       <c r="N12" s="43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O12" s="43" t="s">
         <v>80</v>
       </c>
       <c r="P12" s="43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Q12" s="45"/>
       <c r="R12" s="45"/>
       <c r="S12" s="45"/>
       <c r="T12" s="45"/>
       <c r="U12" s="44" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="V12" s="45"/>
       <c r="W12" s="45"/>
@@ -3454,12 +3470,12 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="51" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C16" s="51"/>
       <c r="D16" s="51"/>
       <c r="E16" s="52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F16" s="52"/>
       <c r="G16" s="52"/>
@@ -3474,7 +3490,7 @@
       <c r="C17" s="53"/>
       <c r="D17" s="53"/>
       <c r="E17" s="54" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
@@ -3489,7 +3505,7 @@
       <c r="C18" s="53"/>
       <c r="D18" s="53"/>
       <c r="E18" s="55" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F18" s="55"/>
       <c r="G18" s="55"/>
@@ -3501,35 +3517,35 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="26" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="25" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="25" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="25" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="25" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="25" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3589,8 +3605,8 @@
   </sheetPr>
   <dimension ref="B1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3598,7 +3614,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="24.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="34.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.63"/>
@@ -3620,7 +3636,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="57" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
@@ -3630,17 +3646,17 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="58" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E4" s="60"/>
       <c r="F4" s="61" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G4" s="61"/>
     </row>
@@ -3648,16 +3664,16 @@
       <c r="B5" s="58"/>
       <c r="C5" s="59"/>
       <c r="D5" s="62" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F5" s="62" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G5" s="62" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3674,10 +3690,10 @@
         <v>79</v>
       </c>
       <c r="F6" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" s="66" t="b">
-        <v>0</v>
+        <v>109</v>
+      </c>
+      <c r="G6" s="66" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3688,16 +3704,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E7" s="41" t="s">
         <v>79</v>
       </c>
       <c r="F7" s="67" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="G7" s="63" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3708,13 +3724,13 @@
         <v>3</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E8" s="41" t="s">
         <v>79</v>
       </c>
       <c r="F8" s="68" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G8" s="63" t="s">
         <v>79</v>
@@ -3731,7 +3747,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="70" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -3750,68 +3766,68 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="73" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C12" s="73"/>
       <c r="D12" s="73"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
       <c r="G12" s="74" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="H12" s="74"/>
       <c r="I12" s="75" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="J12" s="75"/>
       <c r="K12" s="75"/>
       <c r="L12" s="75"/>
       <c r="M12" s="75"/>
       <c r="N12" s="76" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="O12" s="76"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="77" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C13" s="78" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D13" s="78" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E13" s="78"/>
       <c r="F13" s="79" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="80" t="s">
+        <v>124</v>
+      </c>
+      <c r="H13" s="81" t="s">
+        <v>125</v>
+      </c>
+      <c r="I13" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="J13" s="78" t="s">
         <v>120</v>
       </c>
-      <c r="G13" s="80" t="s">
+      <c r="K13" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="H13" s="81" t="s">
-        <v>122</v>
-      </c>
-      <c r="I13" s="77" t="s">
-        <v>123</v>
-      </c>
-      <c r="J13" s="78" t="s">
-        <v>117</v>
-      </c>
-      <c r="K13" s="78" t="s">
-        <v>118</v>
-      </c>
       <c r="L13" s="82" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M13" s="83" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="N13" s="84" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="O13" s="85" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3852,7 +3868,7 @@
         <v>2</v>
       </c>
       <c r="I15" s="92" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="J15" s="87" t="n">
         <v>3</v>
@@ -3867,7 +3883,7 @@
         <v>100</v>
       </c>
       <c r="N15" s="95" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="O15" s="96" t="n">
         <f aca="false">C15</f>

</xml_diff>